<commit_message>
Reformat GDP data format
</commit_message>
<xml_diff>
--- a/data/SG GDP by Industry ANNUAL.xlsx
+++ b/data/SG GDP by Industry ANNUAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MTech EBAC Sem 1\Practice Module\F5-APM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC653A4-C2B9-4019-A590-40EA1FBDA4EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1EADF0-20B3-4D84-A577-6CE06892A7F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="46">
   <si>
     <t xml:space="preserve"> Subject: National Accounts </t>
   </si>
@@ -141,6 +141,24 @@
   </si>
   <si>
     <t xml:space="preserve">Contact: info@singstat.gov.sg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goods Producing Industries </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Services Producing Industries </t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>AGRICULTURE, FISHING AND QUARRYING</t>
   </si>
 </sst>
 </file>
@@ -983,9 +1001,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BI46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="BB13" sqref="BB13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="25.68359375" customWidth="1"/>
+    <col min="2" max="53" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
@@ -5676,753 +5700,577 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9CB1702-3480-4170-B445-056FAEFEE386}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="23.7890625" customWidth="1"/>
+    <col min="2" max="2" width="31.5234375" customWidth="1"/>
+    <col min="3" max="3" width="32.9453125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1">
         <v>2013</v>
       </c>
-      <c r="C1">
+      <c r="E1">
         <v>2014</v>
       </c>
-      <c r="D1">
+      <c r="F1">
         <v>2015</v>
       </c>
-      <c r="E1">
+      <c r="G1">
         <v>2016</v>
       </c>
-      <c r="F1">
+      <c r="H1">
         <v>2017</v>
       </c>
-      <c r="G1">
+      <c r="I1">
         <v>2018</v>
       </c>
-      <c r="H1">
+      <c r="J1">
         <v>2019</v>
       </c>
-      <c r="I1">
+      <c r="K1">
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>4.8</v>
-      </c>
-      <c r="C2">
-        <v>3.9</v>
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>0.3</v>
       </c>
       <c r="E2">
-        <v>3.3</v>
+        <v>0.5</v>
       </c>
       <c r="F2">
-        <v>4.5</v>
+        <v>-0.9</v>
       </c>
       <c r="G2">
-        <v>3.5</v>
+        <v>0.7</v>
       </c>
       <c r="H2">
+        <v>1.8</v>
+      </c>
+      <c r="I2">
         <v>1.3</v>
       </c>
-      <c r="I2">
-        <v>-5.4</v>
+      <c r="J2">
+        <v>-0.3</v>
+      </c>
+      <c r="K2">
+        <v>1.4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>0.5</v>
-      </c>
-      <c r="C3">
-        <v>0.9</v>
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
       <c r="D3">
-        <v>-0.6</v>
+        <v>0.1</v>
       </c>
       <c r="E3">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="F3">
-        <v>1.6</v>
+        <v>0.3</v>
       </c>
       <c r="G3">
-        <v>1.3</v>
+        <v>-0.1</v>
       </c>
       <c r="H3">
         <v>-0.2</v>
       </c>
       <c r="I3">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0.1</v>
+      </c>
+      <c r="K3">
+        <v>-1.3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>0.3</v>
-      </c>
-      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.6</v>
+      </c>
+      <c r="F6">
         <v>0.5</v>
       </c>
-      <c r="D4">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0.3</v>
+      </c>
+      <c r="I6">
+        <v>0.4</v>
+      </c>
+      <c r="J6">
+        <v>-0.1</v>
+      </c>
+      <c r="K6">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0.1</v>
+      </c>
+      <c r="F7">
+        <v>0.1</v>
+      </c>
+      <c r="G7">
+        <v>0.1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>0.2</v>
+      </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+      <c r="F8">
+        <v>0.2</v>
+      </c>
+      <c r="G8">
+        <v>0.1</v>
+      </c>
+      <c r="H8">
+        <v>0.3</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0.1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>0.3</v>
+      </c>
+      <c r="E11">
+        <v>0.3</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0.2</v>
+      </c>
+      <c r="H11">
+        <v>0.3</v>
+      </c>
+      <c r="I11">
+        <v>0.2</v>
+      </c>
+      <c r="J11">
+        <v>0.5</v>
+      </c>
+      <c r="K11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>1.8</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0.5</v>
+      </c>
+      <c r="G12">
+        <v>0.1</v>
+      </c>
+      <c r="H12">
+        <v>0.9</v>
+      </c>
+      <c r="I12">
+        <v>0.7</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>0.4</v>
+      </c>
+      <c r="E13">
+        <v>-0.1</v>
+      </c>
+      <c r="F13">
+        <v>0.1</v>
+      </c>
+      <c r="G13">
+        <v>-0.1</v>
+      </c>
+      <c r="H13">
+        <v>-0.3</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>-0.1</v>
+      </c>
+      <c r="K13">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0.4</v>
+      </c>
+      <c r="G14">
+        <v>0.1</v>
+      </c>
+      <c r="H14">
+        <v>0.2</v>
+      </c>
+      <c r="I14">
+        <v>0.2</v>
+      </c>
+      <c r="J14">
+        <v>0.3</v>
+      </c>
+      <c r="K14">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15">
+        <v>0.3</v>
+      </c>
+      <c r="E15">
+        <v>0.4</v>
+      </c>
+      <c r="F15">
+        <v>0.7</v>
+      </c>
+      <c r="G15">
+        <v>0.7</v>
+      </c>
+      <c r="H15">
+        <v>0.3</v>
+      </c>
+      <c r="I15">
+        <v>0.2</v>
+      </c>
+      <c r="J15">
+        <v>-0.6</v>
+      </c>
+      <c r="K15">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <v>0.2</v>
+      </c>
+      <c r="E16">
+        <v>0.3</v>
+      </c>
+      <c r="F16">
+        <v>0.3</v>
+      </c>
+      <c r="G16">
+        <v>0.4</v>
+      </c>
+      <c r="H16">
+        <v>0.3</v>
+      </c>
+      <c r="I16">
+        <v>0.2</v>
+      </c>
+      <c r="J16">
+        <v>0.4</v>
+      </c>
+      <c r="K16">
         <v>-0.9</v>
-      </c>
-      <c r="E4">
-        <v>0.7</v>
-      </c>
-      <c r="F4">
-        <v>1.8</v>
-      </c>
-      <c r="G4">
-        <v>1.3</v>
-      </c>
-      <c r="H4">
-        <v>-0.3</v>
-      </c>
-      <c r="I4">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>0.1</v>
-      </c>
-      <c r="C5">
-        <v>0.4</v>
-      </c>
-      <c r="D5">
-        <v>0.3</v>
-      </c>
-      <c r="E5">
-        <v>-0.1</v>
-      </c>
-      <c r="F5">
-        <v>-0.2</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0.1</v>
-      </c>
-      <c r="I5">
-        <v>-1.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>4.5</v>
-      </c>
-      <c r="C8">
-        <v>2.9</v>
-      </c>
-      <c r="D8">
-        <v>2.8</v>
-      </c>
-      <c r="E8">
-        <v>1.7</v>
-      </c>
-      <c r="F8">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="G8">
-        <v>2.1</v>
-      </c>
-      <c r="H8">
-        <v>1.3</v>
-      </c>
-      <c r="I8">
-        <v>-4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C9">
-        <v>0.7</v>
-      </c>
-      <c r="D9">
-        <v>0.6</v>
-      </c>
-      <c r="E9">
-        <v>0.1</v>
-      </c>
-      <c r="F9">
-        <v>0.3</v>
-      </c>
-      <c r="G9">
-        <v>0.4</v>
-      </c>
-      <c r="H9">
-        <v>-0.2</v>
-      </c>
-      <c r="I9">
-        <v>-0.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C10">
-        <v>0.6</v>
-      </c>
-      <c r="D10">
-        <v>0.5</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0.3</v>
-      </c>
-      <c r="G10">
-        <v>0.4</v>
-      </c>
-      <c r="H10">
-        <v>-0.1</v>
-      </c>
-      <c r="I10">
-        <v>-0.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0.1</v>
-      </c>
-      <c r="D11">
-        <v>0.1</v>
-      </c>
-      <c r="E11">
-        <v>0.1</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>0.2</v>
-      </c>
-      <c r="C12">
-        <v>0.1</v>
-      </c>
-      <c r="D12">
-        <v>0.2</v>
-      </c>
-      <c r="E12">
-        <v>0.1</v>
-      </c>
-      <c r="F12">
-        <v>0.3</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>-1.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>0.1</v>
-      </c>
-      <c r="C13">
-        <v>0.1</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0.1</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0.1</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0.1</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15">
-        <v>0.1</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>-0.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16">
-        <v>0.3</v>
-      </c>
-      <c r="C16">
-        <v>0.3</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0.2</v>
-      </c>
-      <c r="F16">
-        <v>0.3</v>
-      </c>
-      <c r="G16">
-        <v>0.2</v>
-      </c>
-      <c r="H16">
-        <v>0.5</v>
-      </c>
-      <c r="I16">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17">
-        <v>1.8</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>0.5</v>
-      </c>
-      <c r="E17">
-        <v>0.1</v>
-      </c>
-      <c r="F17">
-        <v>0.9</v>
-      </c>
-      <c r="G17">
-        <v>0.7</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18">
-        <v>0.8</v>
-      </c>
-      <c r="C18">
-        <v>0.4</v>
-      </c>
-      <c r="D18">
-        <v>1.2</v>
-      </c>
-      <c r="E18">
-        <v>0.7</v>
-      </c>
-      <c r="F18">
-        <v>0.2</v>
-      </c>
-      <c r="G18">
-        <v>0.4</v>
-      </c>
-      <c r="H18">
-        <v>-0.3</v>
-      </c>
-      <c r="I18">
-        <v>-1.7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19">
-        <v>0.4</v>
-      </c>
-      <c r="C19">
-        <v>-0.1</v>
-      </c>
-      <c r="D19">
-        <v>0.1</v>
-      </c>
-      <c r="E19">
-        <v>-0.1</v>
-      </c>
-      <c r="F19">
-        <v>-0.3</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>-0.1</v>
-      </c>
-      <c r="I19">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0.4</v>
-      </c>
-      <c r="E20">
-        <v>0.1</v>
-      </c>
-      <c r="F20">
-        <v>0.2</v>
-      </c>
-      <c r="G20">
-        <v>0.2</v>
-      </c>
-      <c r="H20">
-        <v>0.3</v>
-      </c>
-      <c r="I20">
-        <v>-0.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21">
-        <v>0.3</v>
-      </c>
-      <c r="C21">
-        <v>0.4</v>
-      </c>
-      <c r="D21">
-        <v>0.7</v>
-      </c>
-      <c r="E21">
-        <v>0.7</v>
-      </c>
-      <c r="F21">
-        <v>0.3</v>
-      </c>
-      <c r="G21">
-        <v>0.2</v>
-      </c>
-      <c r="H21">
-        <v>-0.6</v>
-      </c>
-      <c r="I21">
-        <v>-0.7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22">
-        <v>0.2</v>
-      </c>
-      <c r="C22">
-        <v>0.3</v>
-      </c>
-      <c r="D22">
-        <v>0.3</v>
-      </c>
-      <c r="E22">
-        <v>0.4</v>
-      </c>
-      <c r="F22">
-        <v>0.3</v>
-      </c>
-      <c r="G22">
-        <v>0.2</v>
-      </c>
-      <c r="H22">
-        <v>0.4</v>
-      </c>
-      <c r="I22">
-        <v>-0.9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23">
-        <v>0.1</v>
-      </c>
-      <c r="C23">
-        <v>0.2</v>
-      </c>
-      <c r="D23">
-        <v>0.2</v>
-      </c>
-      <c r="E23">
-        <v>0.2</v>
-      </c>
-      <c r="F23">
-        <v>0.2</v>
-      </c>
-      <c r="G23">
-        <v>0.2</v>
-      </c>
-      <c r="H23">
-        <v>0.1</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24">
-        <v>-0.2</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0.6</v>
-      </c>
-      <c r="E24">
-        <v>0.8</v>
-      </c>
-      <c r="F24">
-        <v>0.4</v>
-      </c>
-      <c r="G24">
-        <v>-0.1</v>
-      </c>
-      <c r="H24">
-        <v>0.1</v>
-      </c>
-      <c r="I24">
-        <v>-0.9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Produced time series chart for overall and sector GDP
</commit_message>
<xml_diff>
--- a/data/SG GDP by Industry ANNUAL.xlsx
+++ b/data/SG GDP by Industry ANNUAL.xlsx
@@ -2,26 +2,31 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MTech EBAC Sem 1\Practice Module\F5-APM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1EADF0-20B3-4D84-A577-6CE06892A7F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2C7C52-71E6-4BF0-9CC8-CFCA307B2698}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
     <sheet name="Processed" sheetId="2" r:id="rId2"/>
+    <sheet name="SG Overall GDP" sheetId="6" r:id="rId3"/>
+    <sheet name="SG GDP by Sector" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="16" r:id="rId5"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="63">
   <si>
     <t xml:space="preserve"> Subject: National Accounts </t>
   </si>
@@ -159,6 +164,57 @@
   </si>
   <si>
     <t>AGRICULTURE, FISHING AND QUARRYING</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2013Y</t>
+  </si>
+  <si>
+    <t>2014Y</t>
+  </si>
+  <si>
+    <t>2015Y</t>
+  </si>
+  <si>
+    <t>2016Y</t>
+  </si>
+  <si>
+    <t>2017Y</t>
+  </si>
+  <si>
+    <t>2018Y</t>
+  </si>
+  <si>
+    <t>2019Y</t>
+  </si>
+  <si>
+    <t>2020Y</t>
   </si>
 </sst>
 </file>
@@ -642,8 +698,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -700,6 +761,4297 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[SG GDP by Industry ANNUAL.xlsx]SG Overall GDP!PivotTable2</c:name>
+    <c:fmtId val="1"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-SG"/>
+              <a:t>Singapore</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-SG" baseline="0"/>
+              <a:t> Overall GDP (2013 - 2020)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SG Overall GDP'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SG Overall GDP'!$A$4:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SG Overall GDP'!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1999999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.3000000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5680-4330-A7FB-D718771DC5A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2131536384"/>
+        <c:axId val="2131545536"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2131536384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2131545536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2131545536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2131536384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[SG GDP by Industry ANNUAL.xlsx]SG GDP by Sector!PivotTable3</c:name>
+    <c:fmtId val="5"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-SG"/>
+              <a:t>SG GDP by Sector (2013 - 2018)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.1559764861927938E-2"/>
+          <c:y val="0.13668689602820078"/>
+          <c:w val="0.52234986392902005"/>
+          <c:h val="0.82277506524680033"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>         Accommodation &amp; Food Services </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SG GDP by Sector'!$B$5:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-966C-4BC3-BB5E-052ED28653A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>         Construction </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SG GDP by Sector'!$C$5:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-966C-4BC3-BB5E-052ED28653A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$D$3:$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>         Finance &amp; Insurance </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SG GDP by Sector'!$D$5:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-966C-4BC3-BB5E-052ED28653A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$E$3:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>         Information &amp; Communications </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SG GDP by Sector'!$E$5:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-966C-4BC3-BB5E-052ED28653A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$F$3:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>         Manufacturing </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SG GDP by Sector'!$F$5:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-966C-4BC3-BB5E-052ED28653A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$G$3:$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>         Other Goods Industries * </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SG GDP by Sector'!$G$5:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-966C-4BC3-BB5E-052ED28653A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$H$3:$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>         Other Services Industries </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SG GDP by Sector'!$H$5:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-966C-4BC3-BB5E-052ED28653A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$I$3:$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>         Real Estate, Professional Services And Administrative &amp; Support Services </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SG GDP by Sector'!$I$5:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-966C-4BC3-BB5E-052ED28653A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$J$3:$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>         Transportation &amp; Storage </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SG GDP by Sector'!$J$5:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-966C-4BC3-BB5E-052ED28653A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$K$3:$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>         Utilities </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SG GDP by Sector'!$K$5:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-966C-4BC3-BB5E-052ED28653A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$L$3:$L$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>         Wholesale &amp; Retail Trade </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SG GDP by Sector'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SG GDP by Sector'!$L$5:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-966C-4BC3-BB5E-052ED28653A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="163925424"/>
+        <c:axId val="163926672"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="163925424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="163926672"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="163926672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="163925424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.58305142415545586"/>
+          <c:y val="8.1505148670290253E-2"/>
+          <c:w val="0.40732468074664457"/>
+          <c:h val="0.89918594595798296"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>775334</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>62865</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>377189</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>62865</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED3AB3A1-36E1-48C3-B475-6589C4A1D0C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>234314</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>78104</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>87630</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6879D17-3892-4089-A04D-ED500A0D4499}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Sam" refreshedDate="44295.941522453701" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="15" xr:uid="{980AAEBB-90B3-4E4A-8A2E-BA1D74474202}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:K16" sheet="Processed"/>
+  </cacheSource>
+  <cacheFields count="11">
+    <cacheField name="Overview" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Goods Producing Industries "/>
+        <s v="Services Producing Industries "/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Industry" numFmtId="0">
+      <sharedItems count="11">
+        <s v="         Manufacturing "/>
+        <s v="         Construction "/>
+        <s v="         Utilities "/>
+        <s v="         Other Goods Industries * "/>
+        <s v="         Wholesale &amp; Retail Trade "/>
+        <s v="         Transportation &amp; Storage "/>
+        <s v="         Accommodation &amp; Food Services "/>
+        <s v="         Information &amp; Communications "/>
+        <s v="         Finance &amp; Insurance "/>
+        <s v="         Real Estate, Professional Services And Administrative &amp; Support Services "/>
+        <s v="         Other Services Industries "/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Sector" numFmtId="0">
+      <sharedItems count="15">
+        <s v="         Manufacturing "/>
+        <s v="         Construction "/>
+        <s v="         Utilities "/>
+        <s v="AGRICULTURE, FISHING AND QUARRYING"/>
+        <s v="             Wholesale Trade "/>
+        <s v="             Retail Trade "/>
+        <s v="         Transportation &amp; Storage "/>
+        <s v="             Accommodation "/>
+        <s v="             Food &amp; Beverage Services "/>
+        <s v="         Information &amp; Communications "/>
+        <s v="         Finance &amp; Insurance "/>
+        <s v="             Real Estate "/>
+        <s v="             Professional Services "/>
+        <s v="             Administrative &amp; Support Services "/>
+        <s v="         Other Services Industries "/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="2013Y" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="1.8" count="7">
+        <n v="0.3"/>
+        <n v="0.1"/>
+        <n v="0"/>
+        <n v="1.1000000000000001"/>
+        <n v="0.2"/>
+        <n v="1.8"/>
+        <n v="0.4"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="2014Y" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-0.1" maxValue="1"/>
+    </cacheField>
+    <cacheField name="2015Y" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-0.9" maxValue="0.7"/>
+    </cacheField>
+    <cacheField name="2016Y" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-0.1" maxValue="0.7"/>
+    </cacheField>
+    <cacheField name="2017Y" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-0.3" maxValue="1.8"/>
+    </cacheField>
+    <cacheField name="2018Y" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="1.3"/>
+    </cacheField>
+    <cacheField name="2019Y" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-0.6" maxValue="1"/>
+    </cacheField>
+    <cacheField name="2020Y" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1.6" maxValue="1.4"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="15">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="-0.9"/>
+    <n v="0.7"/>
+    <n v="1.8"/>
+    <n v="1.3"/>
+    <n v="-0.3"/>
+    <n v="1.4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.4"/>
+    <n v="0.3"/>
+    <n v="-0.1"/>
+    <n v="-0.2"/>
+    <n v="0"/>
+    <n v="0.1"/>
+    <n v="-1.3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="0.6"/>
+    <n v="0.5"/>
+    <n v="0"/>
+    <n v="0.3"/>
+    <n v="0.4"/>
+    <n v="-0.1"/>
+    <n v="-0.4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="0.1"/>
+    <n v="0.1"/>
+    <n v="0.1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="-0.2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="6"/>
+    <x v="4"/>
+    <n v="0.1"/>
+    <n v="0.2"/>
+    <n v="0.1"/>
+    <n v="0.3"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="-1.6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="7"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0.1"/>
+    <n v="0"/>
+    <n v="-0.2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="8"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="-0.3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="9"/>
+    <x v="0"/>
+    <n v="0.3"/>
+    <n v="0"/>
+    <n v="0.2"/>
+    <n v="0.3"/>
+    <n v="0.2"/>
+    <n v="0.5"/>
+    <n v="0.1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="10"/>
+    <x v="5"/>
+    <n v="1"/>
+    <n v="0.5"/>
+    <n v="0.1"/>
+    <n v="0.9"/>
+    <n v="0.7"/>
+    <n v="1"/>
+    <n v="0.7"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="9"/>
+    <x v="11"/>
+    <x v="6"/>
+    <n v="-0.1"/>
+    <n v="0.1"/>
+    <n v="-0.1"/>
+    <n v="-0.3"/>
+    <n v="0"/>
+    <n v="-0.1"/>
+    <n v="-0.5"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="9"/>
+    <x v="12"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="0.4"/>
+    <n v="0.1"/>
+    <n v="0.2"/>
+    <n v="0.2"/>
+    <n v="0.3"/>
+    <n v="-0.6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="9"/>
+    <x v="13"/>
+    <x v="0"/>
+    <n v="0.4"/>
+    <n v="0.7"/>
+    <n v="0.7"/>
+    <n v="0.3"/>
+    <n v="0.2"/>
+    <n v="-0.6"/>
+    <n v="-0.7"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="14"/>
+    <x v="4"/>
+    <n v="0.3"/>
+    <n v="0.3"/>
+    <n v="0.4"/>
+    <n v="0.3"/>
+    <n v="0.2"/>
+    <n v="0.4"/>
+    <n v="-0.9"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{353697C8-29E8-43C1-B62F-1AA055D5C8B6}" name="PivotTable2" cacheId="16" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="11">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="16">
+        <item x="7"/>
+        <item x="13"/>
+        <item x="8"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="0"/>
+        <item x="14"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="6">
+    <dataField name="2013" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="2014" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="2015" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="2016" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="2017" fld="7" baseField="0" baseItem="0"/>
+    <dataField name="2018" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7D527153-C978-47EC-A9AB-3F8B7B0F0191}" name="PivotTable3" cacheId="16" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A3:M10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="11">
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="12">
+        <item x="6"/>
+        <item x="1"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="8">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="12">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="6">
+    <dataField name="2013" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="2014" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="2015" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="2016" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="2017" fld="7" baseField="0" baseItem="0"/>
+    <dataField name="2018" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="22">
+    <chartFormat chart="1" format="14" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="15" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="16" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="17" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="18" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="20" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="21" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="23" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="24" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5702,8 +10054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9CB1702-3480-4170-B445-056FAEFEE386}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5723,29 +10075,29 @@
       <c r="C1" t="s">
         <v>44</v>
       </c>
-      <c r="D1">
-        <v>2013</v>
-      </c>
-      <c r="E1">
-        <v>2014</v>
-      </c>
-      <c r="F1">
-        <v>2015</v>
-      </c>
-      <c r="G1">
-        <v>2016</v>
-      </c>
-      <c r="H1">
-        <v>2017</v>
-      </c>
-      <c r="I1">
-        <v>2018</v>
-      </c>
-      <c r="J1">
-        <v>2019</v>
-      </c>
-      <c r="K1">
-        <v>2020</v>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6276,4 +10628,400 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07ED18F3-508E-4893-A140-484AD8A05335}">
+  <dimension ref="A3:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="6.1015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="11.734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4.8000000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3.5999999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2.1999999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3.3000000000000007</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409CFE9B-415E-4BCB-8755-54C99FD52913}">
+  <dimension ref="A3:M10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.3671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.3671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="25.3671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="64.3125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.62890625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.20703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.62890625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.20703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M5" s="2">
+        <v>4.8000000000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="M6" s="2">
+        <v>3.5999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>-0.9</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="M7" s="2">
+        <v>2.1999999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M8" s="2">
+        <v>2.1999999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-0.2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="M9" s="2">
+        <v>3.8999999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="M10" s="2">
+        <v>3.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>